<commit_message>
update Descrição e RF
</commit_message>
<xml_diff>
--- a/.Netos/ES2N-Requisitos_Funcionais_dotNetos_.xlsx
+++ b/.Netos/ES2N-Requisitos_Funcionais_dotNetos_.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10668" windowHeight="9000"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
   <si>
     <t xml:space="preserve">LISTA DE REQUISITOS FUNCIONAIS </t>
   </si>
@@ -71,7 +71,7 @@
     <t>Visualizar Resumo do Site e API Google Maps</t>
   </si>
   <si>
-    <t>Esse requisito permite o usuário(Visitante) vizualizar a tela inicial que demonstra um breve resumo da funcionalidade da aplicação e uma pequena janela com a API do Google Maps, que tem visualização completa permitida apenas aos usuários que realizarem seu cadastro. (tela inicial que será apresentada toda vez antes da tela de Login).</t>
+    <t>Esse requisito permite o Usuário vizualizar a tela inicial que demonstra um breve resumo da funcionalidade da aplicação e uma pequena janela com a API do Google Maps, que tem visualização completa permitida apenas aos usuários que realizarem seu cadastro. (tela inicial que será apresentada toda vez antes da tela de Login).</t>
   </si>
   <si>
     <t>Alta</t>
@@ -86,10 +86,10 @@
     <t>Realizar Login</t>
   </si>
   <si>
-    <t>Esse requisito permite aos usuários (todos) acessarem o sistema.</t>
-  </si>
-  <si>
-    <t>Pode executar RF04</t>
+    <t>Esse requisito permite ao Usuário acessarem o sistema.</t>
+  </si>
+  <si>
+    <t>Pode executar RF05</t>
   </si>
   <si>
     <t>RF03</t>
@@ -107,7 +107,7 @@
     <t>Realizar Logout</t>
   </si>
   <si>
-    <t>Esse requisito permite aos usuários (todos) saírem do sistema.</t>
+    <t>Esse requisito permite ao Usuário saírem do sistema.</t>
   </si>
   <si>
     <t>RF05</t>
@@ -116,7 +116,7 @@
     <t>Recuperar Senha</t>
   </si>
   <si>
-    <t>Esse requisito permite aos usuários recuperarem sua
+    <t>Esse requisito permite ao Usuário recuperarem sua
 senha, caso tenham perdido ou esquecido.</t>
   </si>
   <si>
@@ -155,12 +155,12 @@
     <t>Gerenciar Perfil</t>
   </si>
   <si>
-    <t>Este requisito permite aos usuários (todos) que editem as
+    <t>Este requisito permite ao Usuário editar as
 informações de seu perfil, além de poder realizar sua
 exclusão.</t>
   </si>
   <si>
-    <t>Pode executar RF23</t>
+    <t>Pode executar RF22</t>
   </si>
   <si>
     <t>RF09</t>
@@ -181,7 +181,7 @@
     <t>Esse requisito permite ao usuário (Turista) consultar os parques já visitados.</t>
   </si>
   <si>
-    <t>Pode executar RF21, RF25, RF26</t>
+    <t>Pode executar RF20, RF28</t>
   </si>
   <si>
     <t>RF11</t>
@@ -190,7 +190,7 @@
     <t>Validar Gerentes de Parques</t>
   </si>
   <si>
-    <t>Esse requisito permite ao administrador do sistema validar o cadastro de um gerente de um parque.</t>
+    <t>Esse requisito permite ao Administrador do Sistema validar o cadastro de um gerente de um parque.</t>
   </si>
   <si>
     <t>RF12</t>
@@ -310,7 +310,7 @@
     <t>Esse requisito permite ao (Guia) aprovar a oficialização da visita do usuário Turista</t>
   </si>
   <si>
-    <t>Deve chamar RF30</t>
+    <t>Deve chamar RF25</t>
   </si>
   <si>
     <t>RF25</t>
@@ -331,6 +331,9 @@
     <t>Esse requisito permite ao usuário (Gerente) criar equipes para participar de desafios e eventos sazonais</t>
   </si>
   <si>
+    <t>Pode chamar RF25</t>
+  </si>
+  <si>
     <t>RF27</t>
   </si>
   <si>
@@ -355,7 +358,16 @@
     <t>Conversar com guias e gerentes</t>
   </si>
   <si>
-    <t>Esse requisito permite aos usuários (todos) comunicar com os guias e gerentes de determinado parque através de um chat estilo desk</t>
+    <t>Esse requisito permite ao Usuário comunicar com os guias e gerentes de determinado parque através de um chat estilo desk</t>
+  </si>
+  <si>
+    <t>RF30</t>
+  </si>
+  <si>
+    <t>Gerenciar Usuários</t>
+  </si>
+  <si>
+    <t>Esse requisito permite ao Administrador do sistema Validar, Adicionar, Excluir ou Alterar os dados dos demais usuários do sistema.</t>
   </si>
 </sst>
 </file>
@@ -1412,8 +1424,8 @@
   <sheetPr/>
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1504,7 +1516,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" ht="23.4" spans="1:5">
+    <row r="11" ht="64" customHeight="1" spans="1:5">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
@@ -1521,7 +1533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" ht="93.6" spans="1:5">
+    <row r="12" ht="136" customHeight="1" spans="1:5">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
@@ -1630,7 +1642,7 @@
       </c>
       <c r="E18" s="14"/>
     </row>
-    <row r="19" ht="23.4" spans="1:6">
+    <row r="19" ht="51" customHeight="1" spans="1:6">
       <c r="A19" s="12" t="s">
         <v>46</v>
       </c>
@@ -1889,17 +1901,19 @@
       <c r="D35" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="14"/>
+      <c r="E35" s="14" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="36" ht="46.8" spans="1:5">
       <c r="A36" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>15</v>
@@ -1908,13 +1922,13 @@
     </row>
     <row r="37" ht="70.2" spans="1:5">
       <c r="A37" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>38</v>
@@ -1923,18 +1937,33 @@
     </row>
     <row r="38" ht="46.8" spans="1:5">
       <c r="A38" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D38" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E38" s="14"/>
+    </row>
+    <row r="39" ht="46.8" spans="1:5">
+      <c r="A39" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="14"/>
     </row>
     <row r="46" spans="3:5">
       <c r="C46" s="2"/>

</xml_diff>